<commit_message>
moved to shared context so that we could reduce data passing - still more places to remove duplicate data - crunched some new performance numbers.  looking a little better.
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
   <si>
     <t>Cornell Box</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Run Time (ms)</t>
+  </si>
+  <si>
+    <t>OpenCl - GPU</t>
+  </si>
+  <si>
+    <t>C++ (CPU)</t>
   </si>
 </sst>
 </file>
@@ -100,12 +106,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,221 +395,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>75</v>
-      </c>
-      <c r="C3">
-        <v>206</v>
-      </c>
-      <c r="D3">
-        <v>235</v>
-      </c>
-      <c r="E3">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>183</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>121</v>
+      </c>
+      <c r="J4">
+        <v>471</v>
+      </c>
+      <c r="K4">
+        <v>1737</v>
+      </c>
+      <c r="L4">
+        <v>7240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <f>1/(B3/1000)</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4" si="0">1/(C3/1000)</f>
-        <v>4.8543689320388355</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4" si="1">1/(D3/1000)</f>
-        <v>4.2553191489361701</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="2">1/(E3/1000)</f>
-        <v>2.1645021645021645</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B5">
+        <f>1/(B4/1000)</f>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5" si="0">1/(C4/1000)</f>
+        <v>76.92307692307692</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5" si="1">1/(D4/1000)</f>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5" si="2">1/(E4/1000)</f>
+        <v>5.4644808743169397</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <f>1/(I4/1000)</f>
+        <v>8.2644628099173563</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:L5" si="3">1/(J4/1000)</f>
+        <v>2.1231422505307855</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>0.57570523891767411</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>0.13812154696132597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>193</v>
-      </c>
-      <c r="C8">
-        <v>178</v>
-      </c>
-      <c r="D8">
-        <v>290</v>
-      </c>
-      <c r="E8">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>99</v>
+      </c>
+      <c r="E9">
+        <v>333</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>97</v>
+      </c>
+      <c r="J9">
+        <v>375</v>
+      </c>
+      <c r="K9">
+        <v>1459</v>
+      </c>
+      <c r="L9">
+        <v>5521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
-        <f>1/(B8/1000)</f>
-        <v>5.1813471502590671</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9" si="3">1/(C8/1000)</f>
-        <v>5.617977528089888</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9" si="4">1/(D8/1000)</f>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9" si="5">1/(E8/1000)</f>
-        <v>1.7211703958691911</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B10">
+        <f>1/(B9/1000)</f>
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10" si="4">1/(C9/1000)</f>
+        <v>34.482758620689651</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10" si="5">1/(D9/1000)</f>
+        <v>10.1010101010101</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10" si="6">1/(E9/1000)</f>
+        <v>3.0030030030030028</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <f>1/(I9/1000)</f>
+        <v>10.309278350515463</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:L10" si="7">1/(J9/1000)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>0.68540095956134339</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="7"/>
+        <v>0.18112660749864154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>384</v>
-      </c>
-      <c r="C13">
-        <v>465</v>
-      </c>
-      <c r="D13">
-        <v>855</v>
-      </c>
-      <c r="E13">
-        <v>2153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>118</v>
+      </c>
+      <c r="D14">
+        <v>468</v>
+      </c>
+      <c r="E14">
+        <v>1580</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B14">
-        <f>1/(B13/1000)</f>
-        <v>2.6041666666666665</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ref="C14:E14" si="6">1/(C13/1000)</f>
-        <v>2.150537634408602</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="6"/>
-        <v>1.1695906432748537</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="6"/>
-        <v>0.46446818392940081</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15">
+        <f>1/(B14/1000)</f>
+        <v>29.411764705882351</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:E15" si="8">1/(C14/1000)</f>
+        <v>8.4745762711864412</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="8"/>
+        <v>2.1367521367521367</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="8"/>
+        <v>0.63291139240506322</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="e">
+        <f>1/(I14/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" t="e">
+        <f t="shared" ref="J15:L15" si="9">1/(J14/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
stupid changes that it won't revert
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\openclraytracer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sturgedl\Documents\git\openclraytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -109,10 +109,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -398,7 +398,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F1" sqref="F1:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,38 +408,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -546,20 +546,20 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -666,20 +666,20 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="H12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="H12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -780,14 +780,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H1:L1"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="H1:L1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
added lots of awesome image files...
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
-  <si>
-    <t>Cornell Box</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="12">
   <si>
     <t>Resolution</t>
   </si>
@@ -44,15 +41,6 @@
     <t>2048x2048</t>
   </si>
   <si>
-    <t>Blue Sphere</t>
-  </si>
-  <si>
-    <t>Dragon</t>
-  </si>
-  <si>
-    <t>Run times are averaged time of 25 rendered frames.</t>
-  </si>
-  <si>
     <t>FPS</t>
   </si>
   <si>
@@ -63,12 +51,24 @@
   </si>
   <si>
     <t>C++ (CPU)</t>
+  </si>
+  <si>
+    <t>Cornell Box - 30 Triangles</t>
+  </si>
+  <si>
+    <t>Blue Sphere - 970 Triangles</t>
+  </si>
+  <si>
+    <t>Dragon - ~870k Triangles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,13 +106,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -395,67 +398,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J15"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3" t="s">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" t="s">
         <v>0</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
       </c>
       <c r="H3" t="s">
         <v>1</v>
@@ -469,13 +484,12 @@
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -489,93 +503,111 @@
       <c r="E4">
         <v>183</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
+      <c r="F4" s="4"/>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>121</v>
       </c>
       <c r="I4">
-        <v>121</v>
+        <v>471</v>
       </c>
       <c r="J4">
-        <v>471</v>
+        <v>1737</v>
       </c>
       <c r="K4">
-        <v>1737</v>
-      </c>
-      <c r="L4">
         <v>7240</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
         <f>1/(B4/1000)</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f t="shared" ref="C5" si="0">1/(C4/1000)</f>
         <v>76.92307692307692</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f t="shared" ref="D5" si="1">1/(D4/1000)</f>
         <v>22.222222222222221</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <f t="shared" ref="E5" si="2">1/(E4/1000)</f>
         <v>5.4644808743169397</v>
       </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <f>1/(I4/1000)</f>
+      <c r="F5" s="4"/>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3">
+        <f>1/(H4/1000)</f>
         <v>8.2644628099173563</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:L5" si="3">1/(J4/1000)</f>
+      <c r="I5" s="3">
+        <f t="shared" ref="I5:K5" si="3">1/(I4/1000)</f>
         <v>2.1231422505307855</v>
       </c>
-      <c r="K5">
+      <c r="J5" s="3">
         <f t="shared" si="3"/>
         <v>0.57570523891767411</v>
       </c>
-      <c r="L5">
+      <c r="K5" s="3">
         <f t="shared" si="3"/>
         <v>0.13812154696132597</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>5</v>
+      <c r="F8" s="4"/>
+      <c r="G8" t="s">
+        <v>0</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
@@ -589,13 +621,12 @@
       <c r="K8" t="s">
         <v>4</v>
       </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -609,93 +640,111 @@
       <c r="E9">
         <v>333</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
+      <c r="F9" s="4"/>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>97</v>
       </c>
       <c r="I9">
-        <v>97</v>
+        <v>375</v>
       </c>
       <c r="J9">
-        <v>375</v>
+        <v>1459</v>
       </c>
       <c r="K9">
-        <v>1459</v>
-      </c>
-      <c r="L9">
         <v>5521</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
         <f>1/(B9/1000)</f>
         <v>100</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <f t="shared" ref="C10" si="4">1/(C9/1000)</f>
         <v>34.482758620689651</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <f t="shared" ref="D10" si="5">1/(D9/1000)</f>
         <v>10.1010101010101</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <f t="shared" ref="E10" si="6">1/(E9/1000)</f>
         <v>3.0030030030030028</v>
       </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10">
-        <f>1/(I9/1000)</f>
+      <c r="F10" s="4"/>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <f>1/(H9/1000)</f>
         <v>10.309278350515463</v>
       </c>
-      <c r="J10">
-        <f t="shared" ref="J10:L10" si="7">1/(J9/1000)</f>
+      <c r="I10" s="3">
+        <f t="shared" ref="I10:K10" si="7">1/(I9/1000)</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="K10">
+      <c r="J10" s="3">
         <f t="shared" si="7"/>
         <v>0.68540095956134339</v>
       </c>
-      <c r="L10">
+      <c r="K10" s="3">
         <f t="shared" si="7"/>
         <v>0.18112660749864154</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
-        <v>5</v>
+      <c r="F13" s="4"/>
+      <c r="G13" t="s">
+        <v>0</v>
       </c>
       <c r="H13" t="s">
         <v>1</v>
@@ -709,13 +758,12 @@
       <c r="K13" t="s">
         <v>4</v>
       </c>
-      <c r="L13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>34</v>
@@ -729,67 +777,128 @@
       <c r="E14">
         <v>1580</v>
       </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>1248</v>
+      </c>
+      <c r="I14">
+        <v>8630</v>
+      </c>
+      <c r="J14">
+        <v>32183</v>
+      </c>
+      <c r="K14">
+        <v>122429</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
         <f>1/(B14/1000)</f>
         <v>29.411764705882351</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <f t="shared" ref="C15:E15" si="8">1/(C14/1000)</f>
         <v>8.4745762711864412</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <f t="shared" si="8"/>
         <v>2.1367521367521367</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <f t="shared" si="8"/>
         <v>0.63291139240506322</v>
       </c>
-      <c r="H15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" t="e">
-        <f>1/(I14/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" t="e">
-        <f t="shared" ref="J15:L15" si="9">1/(J14/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" t="e">
+      <c r="F15" s="4"/>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <f>1/(H14/1000)</f>
+        <v>0.80128205128205132</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" ref="I15:K15" si="9">1/(I14/1000)</f>
+        <v>0.11587485515643105</v>
+      </c>
+      <c r="J15" s="3">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" t="e">
+        <v>3.1072305254326818E-2</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
+        <v>8.1679994119040426E-3</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H1:L1"/>
+  <mergeCells count="11">
+    <mergeCell ref="A16:K18"/>
+    <mergeCell ref="L1:M18"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A12:E12"/>
+    <mergeCell ref="F1:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated performance results - the old values were pretty unreasonable compared to what my desktop did.  =(
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sturgedl\Documents\git\openclraytracer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\openclraytracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -108,14 +108,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -400,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:K2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,42 +415,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -468,7 +468,7 @@
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="2"/>
       <c r="G3" t="s">
         <v>0</v>
       </c>
@@ -484,8 +484,8 @@
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -503,7 +503,7 @@
       <c r="E4">
         <v>183</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="2"/>
       <c r="G4" t="s">
         <v>6</v>
       </c>
@@ -519,75 +519,75 @@
       <c r="K4">
         <v>7240</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <f>1/(B4/1000)</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <f t="shared" ref="C5" si="0">1/(C4/1000)</f>
         <v>76.92307692307692</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <f t="shared" ref="D5" si="1">1/(D4/1000)</f>
         <v>22.222222222222221</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <f t="shared" ref="E5" si="2">1/(E4/1000)</f>
         <v>5.4644808743169397</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="2"/>
       <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="1">
         <f>1/(H4/1000)</f>
         <v>8.2644628099173563</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="1">
         <f t="shared" ref="I5:K5" si="3">1/(I4/1000)</f>
         <v>2.1231422505307855</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="1">
         <f t="shared" si="3"/>
         <v>0.57570523891767411</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="1">
         <f t="shared" si="3"/>
         <v>0.13812154696132597</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F6" s="4"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -605,7 +605,7 @@
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="2"/>
       <c r="G8" t="s">
         <v>0</v>
       </c>
@@ -621,8 +621,8 @@
       <c r="K8" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -640,7 +640,7 @@
       <c r="E9">
         <v>333</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="2"/>
       <c r="G9" t="s">
         <v>6</v>
       </c>
@@ -656,75 +656,75 @@
       <c r="K9">
         <v>5521</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <f>1/(B9/1000)</f>
         <v>100</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <f t="shared" ref="C10" si="4">1/(C9/1000)</f>
         <v>34.482758620689651</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <f t="shared" ref="D10" si="5">1/(D9/1000)</f>
         <v>10.1010101010101</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <f t="shared" ref="E10" si="6">1/(E9/1000)</f>
         <v>3.0030030030030028</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="2"/>
       <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="1">
         <f>1/(H9/1000)</f>
         <v>10.309278350515463</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="1">
         <f t="shared" ref="I10:K10" si="7">1/(I9/1000)</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="1">
         <f t="shared" si="7"/>
         <v>0.68540095956134339</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="1">
         <f t="shared" si="7"/>
         <v>0.18112660749864154</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F11" s="4"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="1" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -742,7 +742,7 @@
       <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="2"/>
       <c r="G13" t="s">
         <v>0</v>
       </c>
@@ -758,8 +758,8 @@
       <c r="K13" t="s">
         <v>4</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -777,112 +777,112 @@
       <c r="E14">
         <v>1580</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="2"/>
       <c r="G14" t="s">
         <v>6</v>
       </c>
       <c r="H14">
-        <v>1248</v>
+        <v>185</v>
       </c>
       <c r="I14">
-        <v>8630</v>
+        <v>648</v>
       </c>
       <c r="J14">
-        <v>32183</v>
+        <v>2311</v>
       </c>
       <c r="K14">
-        <v>122429</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+        <v>8323</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <f>1/(B14/1000)</f>
         <v>29.411764705882351</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1">
         <f t="shared" ref="C15:E15" si="8">1/(C14/1000)</f>
         <v>8.4745762711864412</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <f t="shared" si="8"/>
         <v>2.1367521367521367</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <f t="shared" si="8"/>
         <v>0.63291139240506322</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="2"/>
       <c r="G15" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="1">
         <f>1/(H14/1000)</f>
-        <v>0.80128205128205132</v>
-      </c>
-      <c r="I15" s="3">
+        <v>5.4054054054054053</v>
+      </c>
+      <c r="I15" s="1">
         <f t="shared" ref="I15:K15" si="9">1/(I14/1000)</f>
-        <v>0.11587485515643105</v>
-      </c>
-      <c r="J15" s="3">
+        <v>1.5432098765432098</v>
+      </c>
+      <c r="J15" s="1">
         <f t="shared" si="9"/>
-        <v>3.1072305254326818E-2</v>
-      </c>
-      <c r="K15" s="3">
+        <v>0.43271311120726957</v>
+      </c>
+      <c r="K15" s="1">
         <f t="shared" si="9"/>
-        <v>8.1679994119040426E-3</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+        <v>0.12014898474107893</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>